<commit_message>
refining readme and MLR outputs
</commit_message>
<xml_diff>
--- a/Output/pval_table.xlsx
+++ b/Output/pval_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbtyers\Documents\current projects\culvert_stability\Output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbtyers\Documents\Current Projects\culvert_stability\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85443262-20A3-4229-9B51-9F8A994723D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F66635F-D494-459A-B8D1-9337603224D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29655" yWindow="975" windowWidth="19200" windowHeight="11265" xr2:uid="{CCEFD675-45B3-40B6-B5F8-500A4146E0F5}"/>
+    <workbookView xWindow="405" yWindow="2355" windowWidth="27960" windowHeight="12735" xr2:uid="{CCEFD675-45B3-40B6-B5F8-500A4146E0F5}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_pvaltable" sheetId="1" r:id="rId1"/>
@@ -1295,17 +1295,17 @@
   <dimension ref="A1:AG39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AH7" sqref="AH7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="33" width="5.1796875" customWidth="1"/>
+    <col min="1" max="1" width="46.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="33" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>97</v>
       </c>
@@ -1322,7 +1322,7 @@
       </c>
       <c r="AG1" s="2"/>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>101</v>
       </c>
@@ -1351,7 +1351,7 @@
       </c>
       <c r="AG2" s="2"/>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>103</v>
       </c>
@@ -1404,7 +1404,7 @@
       </c>
       <c r="AG3" s="2"/>
     </row>
-    <row r="4" spans="1:33" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>105</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>0.93635868580405501</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1704,7 +1704,7 @@
         <v>0.71830249850729799</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>9.3569737455035598E-8</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>4.6559391690506199E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>0.13430800858969999</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>4.81643703844164E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>0.31124125874679798</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>0.21452606556227199</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>0.59631268236397905</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>0.34368575992275102</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>0.75134817895591199</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -2714,7 +2714,7 @@
         <v>0.62304954584683403</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -2815,7 +2815,7 @@
         <v>5.6084527354243298E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -2916,7 +2916,7 @@
         <v>0.85317949896995504</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>0.54120136893723303</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -3118,7 +3118,7 @@
         <v>1.5768049917433101E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -3219,7 +3219,7 @@
         <v>0.74060487446374701</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -3320,7 +3320,7 @@
         <v>6.3647915514229797E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>52</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>0.44837866100146601</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -3522,7 +3522,7 @@
         <v>7.0257256523189801E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>58</v>
       </c>
@@ -3623,7 +3623,7 @@
         <v>8.8478569883215903E-7</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>59</v>
       </c>
@@ -3724,7 +3724,7 @@
         <v>0.61046577017554104</v>
       </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>64</v>
       </c>
@@ -3825,7 +3825,7 @@
         <v>0.76361916406077102</v>
       </c>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>65</v>
       </c>
@@ -3926,7 +3926,7 @@
         <v>0.95786160929906705</v>
       </c>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>66</v>
       </c>
@@ -4027,7 +4027,7 @@
         <v>0.36194572236383299</v>
       </c>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>67</v>
       </c>
@@ -4128,7 +4128,7 @@
         <v>0.77284807252254695</v>
       </c>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>71</v>
       </c>
@@ -4229,7 +4229,7 @@
         <v>0.43883565535838598</v>
       </c>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>78</v>
       </c>
@@ -4330,7 +4330,7 @@
         <v>0.54381311588332903</v>
       </c>
     </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>82</v>
       </c>
@@ -4431,7 +4431,7 @@
         <v>0.86379461155663795</v>
       </c>
     </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>83</v>
       </c>
@@ -4532,7 +4532,7 @@
         <v>0.499350062901948</v>
       </c>
     </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>86</v>
       </c>
@@ -4633,7 +4633,7 @@
         <v>3.6624169415013202E-4</v>
       </c>
     </row>
-    <row r="36" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>87</v>
       </c>
@@ -4734,7 +4734,7 @@
         <v>0.108991042288076</v>
       </c>
     </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>90</v>
       </c>
@@ -4835,7 +4835,7 @@
         <v>9.2610825003932501E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>92</v>
       </c>
@@ -4936,7 +4936,7 @@
         <v>0.202642521370204</v>
       </c>
     </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>95</v>
       </c>

</xml_diff>